<commit_message>
ExcelDataSourceFile functionality moved to seperate file
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4ED92C-1F10-41E9-96E1-1D1E96F9E778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A7A8D3-6DDC-4B48-BC39-6E600D96EE45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4185" yWindow="3210" windowWidth="28800" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37620" yWindow="1035" windowWidth="28800" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -377,44 +377,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="F1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F1" sqref="F1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel reading tests updated
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C392B1-F4CA-4057-A405-12E00AF92ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE25D0-C8BE-4243-BD7E-B2DC10A709CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2562" yWindow="2562" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>header1</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F1:H3"/>
+  <dimension ref="F1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -444,6 +444,17 @@
       </c>
       <c r="H3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="6:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -455,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E65FFAD-4F56-43F0-A853-F2309E498BE5}">
   <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
bug in AddRow corrected
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE25D0-C8BE-4243-BD7E-B2DC10A709CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7058E683-ABCA-4B9B-93CE-FFB7B1C20ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3084" yWindow="1092" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,49 +45,49 @@
     <t>header3</t>
   </si>
   <si>
+    <t>str2</t>
+  </si>
+  <si>
+    <t>str3</t>
+  </si>
+  <si>
+    <t>str5</t>
+  </si>
+  <si>
+    <t>str6</t>
+  </si>
+  <si>
+    <t>str7</t>
+  </si>
+  <si>
+    <t>str8</t>
+  </si>
+  <si>
+    <t>str9</t>
+  </si>
+  <si>
+    <t>str10</t>
+  </si>
+  <si>
+    <t>str11</t>
+  </si>
+  <si>
+    <t>str12</t>
+  </si>
+  <si>
+    <t>sheet2_header1</t>
+  </si>
+  <si>
+    <t>sheet2_header2</t>
+  </si>
+  <si>
+    <t>sheet2_header3</t>
+  </si>
+  <si>
     <t>str1</t>
   </si>
   <si>
-    <t>str2</t>
-  </si>
-  <si>
-    <t>str3</t>
-  </si>
-  <si>
     <t>str4</t>
-  </si>
-  <si>
-    <t>str5</t>
-  </si>
-  <si>
-    <t>str6</t>
-  </si>
-  <si>
-    <t>str7</t>
-  </si>
-  <si>
-    <t>str8</t>
-  </si>
-  <si>
-    <t>str9</t>
-  </si>
-  <si>
-    <t>str10</t>
-  </si>
-  <si>
-    <t>str11</t>
-  </si>
-  <si>
-    <t>str12</t>
-  </si>
-  <si>
-    <t>sheet2_header1</t>
-  </si>
-  <si>
-    <t>sheet2_header2</t>
-  </si>
-  <si>
-    <t>sheet2_header3</t>
   </si>
 </sst>
 </file>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -426,35 +426,35 @@
     </row>
     <row r="2" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -466,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E65FFAD-4F56-43F0-A853-F2309E498BE5}">
   <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -479,35 +479,35 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unit tests dor ExcelReader added
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7058E683-ABCA-4B9B-93CE-FFB7B1C20ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFDDA48-BB3A-406C-883D-D935FA523B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3084" yWindow="1092" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="1428" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="F1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
test for measurement level added
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFDDA48-BB3A-406C-883D-D935FA523B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395670A-7CD7-4965-9B5A-BEAD3143413D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1428" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="1428" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>header1</t>
   </si>
@@ -66,28 +66,22 @@
     <t>str9</t>
   </si>
   <si>
-    <t>str10</t>
-  </si>
-  <si>
     <t>str11</t>
   </si>
   <si>
-    <t>str12</t>
-  </si>
-  <si>
-    <t>sheet2_header1</t>
-  </si>
-  <si>
-    <t>sheet2_header2</t>
-  </si>
-  <si>
-    <t>sheet2_header3</t>
-  </si>
-  <si>
     <t>str1</t>
   </si>
   <si>
     <t>str4</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -407,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -426,7 +420,7 @@
     </row>
     <row r="2" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -437,7 +431,7 @@
     </row>
     <row r="3" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -466,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E65FFAD-4F56-43F0-A853-F2309E498BE5}">
   <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -489,24 +483,24 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>0.76</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
+      <c r="D2">
+        <v>1700</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1.2</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tests added for levels and existingValues
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395670A-7CD7-4965-9B5A-BEAD3143413D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A82168-773B-493F-9C27-A3C372B3E69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1428" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>header1</t>
   </si>
@@ -82,6 +83,21 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>sheet2_header1</t>
+  </si>
+  <si>
+    <t>sheet2_header2</t>
+  </si>
+  <si>
+    <t>sheet2_header3</t>
+  </si>
+  <si>
+    <t>str10</t>
+  </si>
+  <si>
+    <t>str12</t>
   </si>
 </sst>
 </file>
@@ -460,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E65FFAD-4F56-43F0-A853-F2309E498BE5}">
   <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -473,34 +489,82 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2">
-        <v>0.76</v>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>1700</v>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3">
-        <v>1.2</v>
+      <c r="B3" t="s">
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC1122-9687-4AD1-906B-9DDDA353C07C}">
+  <dimension ref="C1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2">
+        <v>0.76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3">
+        <v>1.2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tests for different cultures added for the parsing of csv doubles
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A82168-773B-493F-9C27-A3C372B3E69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BA8B68-C723-434C-98A2-46827C7B05F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,13 +104,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +537,13 @@
   <dimension ref="C1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="37.20703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
@@ -548,7 +558,7 @@
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C2">
-        <v>0.76</v>
+        <v>3.4101243963859801E-4</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -557,9 +567,9 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3">
-        <v>1.2</v>
+    <row r="3" spans="3:5" ht="17.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="1">
+        <v>34.439998626708899</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -570,5 +580,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test added for excel reading precision - still red
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BA8B68-C723-434C-98A2-46827C7B05F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B3638C-DC37-4BB7-AD6A-BA5E7A099E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="1428" windowWidth="17280" windowHeight="8994" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>header1</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>str12</t>
+  </si>
+  <si>
+    <t>0.000341012439638598</t>
   </si>
 </sst>
 </file>
@@ -141,7 +144,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +540,7 @@
   <dimension ref="C1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -557,8 +560,8 @@
       </c>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2">
-        <v>3.4101243963859801E-4</v>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
considertion for LLOQ added
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B3638C-DC37-4BB7-AD6A-BA5E7A099E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AB121F-5894-4D6D-815E-B0FE34FA76E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1428" windowWidth="17280" windowHeight="8994" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>header1</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>0.000341012439638598</t>
+  </si>
+  <si>
+    <t>lloq</t>
+  </si>
+  <si>
+    <t>&lt;0.01</t>
+  </si>
+  <si>
+    <t>2.23</t>
   </si>
 </sst>
 </file>
@@ -537,10 +546,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC1122-9687-4AD1-906B-9DDDA353C07C}">
-  <dimension ref="C1:E3"/>
+  <dimension ref="C1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -548,7 +557,7 @@
     <col min="3" max="3" width="37.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -558,8 +567,11 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -569,8 +581,11 @@
       <c r="E2">
         <v>1700</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" ht="17.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="1">
         <v>34.439998626708899</v>
       </c>
@@ -579,6 +594,9 @@
       </c>
       <c r="E3">
         <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for parsing NaN added
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AB121F-5894-4D6D-815E-B0FE34FA76E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8154EC89-7E13-4654-A0CF-BAA9B3002BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>header1</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>2.23</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -546,18 +552,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC1122-9687-4AD1-906B-9DDDA353C07C}">
-  <dimension ref="C1:F3"/>
+  <dimension ref="C1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="37.20703125" customWidth="1"/>
+    <col min="7" max="7" width="16.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -570,8 +577,11 @@
       <c r="F1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -584,8 +594,11 @@
       <c r="F2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="3:6" ht="17.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="1">
         <v>34.439998626708899</v>
       </c>
@@ -597,6 +610,9 @@
       </c>
       <c r="F3" t="s">
         <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug with empty values in last column fixed
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8154EC89-7E13-4654-A0CF-BAA9B3002BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350D9204-5F14-4328-8050-BB7554034C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="18840" windowHeight="13635" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>header1</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>empty row</t>
   </si>
 </sst>
 </file>
@@ -446,9 +449,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="6:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="6:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>11</v>
       </c>
@@ -470,7 +473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="6:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>12</v>
       </c>
@@ -481,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="6:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>7</v>
       </c>
@@ -502,17 +505,17 @@
   <dimension ref="B1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.68359375" customWidth="1"/>
-    <col min="3" max="3" width="19.41796875" customWidth="1"/>
-    <col min="4" max="4" width="21.9453125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -523,7 +526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -534,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -552,19 +555,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC1122-9687-4AD1-906B-9DDDA353C07C}">
-  <dimension ref="C1:G3"/>
+  <dimension ref="C1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H1" sqref="H1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.20703125" customWidth="1"/>
-    <col min="7" max="7" width="16.734375" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -580,8 +584,11 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -598,7 +605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="3:7" ht="17.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="3:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>34.439998626708899</v>
       </c>
@@ -613,6 +620,9 @@
       </c>
       <c r="G3" t="s">
         <v>26</v>
+      </c>
+      <c r="H3">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
678 importing cells with formula (#1473)
* building

* updating npoi

* updating nugfet depndencies

* correcting not supported formula

* unit test added

* appvezor.yml corrected

* unit test cortrected
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/sample1.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350D9204-5F14-4328-8050-BB7554034C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD79B264-D77A-4AA3-B24E-DF0633A94E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18840" windowHeight="13635" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>header1</t>
   </si>
@@ -119,6 +120,18 @@
   </si>
   <si>
     <t>empty row</t>
+  </si>
+  <si>
+    <t>Concat_test1</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Concat_test2</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -449,9 +462,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" t="s">
         <v>11</v>
       </c>
@@ -473,7 +486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" t="s">
         <v>12</v>
       </c>
@@ -484,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" t="s">
         <v>7</v>
       </c>
@@ -508,14 +521,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.68359375" customWidth="1"/>
+    <col min="3" max="3" width="19.41796875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -526,7 +539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -537,7 +550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -557,18 +570,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC1122-9687-4AD1-906B-9DDDA353C07C}">
   <dimension ref="C1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.15625" customWidth="1"/>
+    <col min="7" max="7" width="16.68359375" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -588,7 +601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -605,7 +618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="3:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="1">
         <v>34.439998626708899</v>
       </c>
@@ -629,4 +642,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C17311C-0A40-4BAB-8FD6-B2F610792588}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>